<commit_message>
Brazil 2000 and updated values
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/size_modifier.xlsx
+++ b/Modding resources/economy spreadsheets/size_modifier.xlsx
@@ -593,36 +593,36 @@
   <dimension ref="A1:X303"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B71" activeCellId="0" sqref="B71"/>
+      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.1813953488372"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.16744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.68837209302326"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.06976744186047"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="4.62790697674419"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.13488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.22790697674419"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.293023255814"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.8418604651163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.293023255814"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.553488372093"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="3.81395348837209"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.27441860465116"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="4.67441860465116"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.16744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.98139534883721"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.3348837209302"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.8"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="3.93953488372093"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="1" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.4604651162791"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="1" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="13.906976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,13 +1246,25 @@
         <v>38</v>
       </c>
       <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
+      <c r="C19" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="H19" s="0"/>
-      <c r="I19" s="0"/>
+      <c r="I19" s="0" t="n">
+        <v>19</v>
+      </c>
       <c r="J19" s="4"/>
       <c r="K19" s="0"/>
       <c r="L19" s="0"/>

</xml_diff>

<commit_message>
ARG MEX USA CAN 2000 industry and biofuel
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/size_modifier.xlsx
+++ b/Modding resources/economy spreadsheets/size_modifier.xlsx
@@ -595,34 +595,34 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6744186046512"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.4"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.38604651162791"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="4.67441860465116"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.49302325581395"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.98139534883721"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.8"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="3.93953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.73953488372093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="4.06046511627907"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="1" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.706976744186"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="1" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.2"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="14.2744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,13 +792,25 @@
         <v>23</v>
       </c>
       <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
-      <c r="E4" s="0"/>
-      <c r="F4" s="0"/>
-      <c r="G4" s="0"/>
+      <c r="C4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="H4" s="0"/>
-      <c r="I4" s="0"/>
+      <c r="I4" s="0" t="n">
+        <v>16</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
@@ -876,13 +888,25 @@
         <v>26</v>
       </c>
       <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
+      <c r="C7" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
+      <c r="I7" s="0" t="n">
+        <v>17</v>
+      </c>
       <c r="J7" s="4"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
@@ -1314,13 +1338,25 @@
         <v>40</v>
       </c>
       <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
-      <c r="E21" s="0"/>
-      <c r="F21" s="0"/>
-      <c r="G21" s="0"/>
+      <c r="C21" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="H21" s="0"/>
-      <c r="I21" s="0"/>
+      <c r="I21" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="J21" s="4"/>
       <c r="K21" s="0"/>
       <c r="L21" s="0"/>
@@ -1398,13 +1434,25 @@
         <v>43</v>
       </c>
       <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="0"/>
-      <c r="F24" s="0"/>
-      <c r="G24" s="0"/>
+      <c r="C24" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="H24" s="0"/>
-      <c r="I24" s="0"/>
+      <c r="I24" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="J24" s="4"/>
       <c r="K24" s="0"/>
       <c r="L24" s="0"/>

</xml_diff>

<commit_message>
Taiwan claims on china
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/size_modifier.xlsx
+++ b/Modding resources/economy spreadsheets/size_modifier.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="189">
   <si>
     <t>Name</t>
   </si>
@@ -467,6 +467,27 @@
   </si>
   <si>
     <t>drc</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>australia</t>
+  </si>
+  <si>
+    <t>turkey</t>
+  </si>
+  <si>
+    <t>uk shipyards</t>
+  </si>
+  <si>
+    <t>greece</t>
+  </si>
+  <si>
+    <t>italy shipyards and mils</t>
+  </si>
+  <si>
+    <t>taiwan add stuff</t>
   </si>
   <si>
     <t>Israel</t>
@@ -695,39 +716,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X337"/>
+  <dimension ref="A1:X343"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G133" activeCellId="0" sqref="G133"/>
+      <selection pane="bottomLeft" activeCell="B129" activeCellId="0" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.6604651162791"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.13953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.50697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.62790697674419"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="4.67441860465116"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.98139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.47441860465116"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.293023255814"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.153488372093"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="4.06046511627907"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="1" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="11.446511627907"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="1" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="15.0139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5667,6 +5688,9 @@
       <c r="A129" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="B129" s="0" t="s">
+        <v>61</v>
+      </c>
       <c r="C129" s="2" t="n">
         <v>11</v>
       </c>
@@ -5984,14 +6008,27 @@
       <c r="X137" s="0"/>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0"/>
-      <c r="C138" s="0"/>
-      <c r="D138" s="0"/>
-      <c r="E138" s="0"/>
+      <c r="A138" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D138" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E138" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="F138" s="0"/>
       <c r="G138" s="0"/>
       <c r="H138" s="0"/>
-      <c r="I138" s="0"/>
+      <c r="I138" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="J138" s="0"/>
       <c r="K138" s="0"/>
       <c r="L138" s="0"/>
@@ -6008,14 +6045,27 @@
       <c r="X138" s="0"/>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0"/>
-      <c r="C139" s="0"/>
-      <c r="D139" s="0"/>
-      <c r="E139" s="0"/>
+      <c r="A139" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D139" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E139" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="F139" s="0"/>
       <c r="G139" s="0"/>
       <c r="H139" s="0"/>
-      <c r="I139" s="0"/>
+      <c r="I139" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="J139" s="0"/>
       <c r="K139" s="0"/>
       <c r="L139" s="0"/>
@@ -6032,14 +6082,25 @@
       <c r="X139" s="0"/>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0"/>
-      <c r="C140" s="0"/>
-      <c r="D140" s="0"/>
-      <c r="E140" s="0"/>
+      <c r="A140" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B140" s="0"/>
+      <c r="C140" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D140" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E140" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="F140" s="0"/>
       <c r="G140" s="0"/>
       <c r="H140" s="0"/>
-      <c r="I140" s="0"/>
+      <c r="I140" s="0" t="n">
+        <v>15</v>
+      </c>
       <c r="J140" s="0"/>
       <c r="K140" s="0"/>
       <c r="L140" s="0"/>
@@ -6056,7 +6117,10 @@
       <c r="X140" s="0"/>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0"/>
+      <c r="A141" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B141" s="0"/>
       <c r="C141" s="0"/>
       <c r="D141" s="0"/>
       <c r="E141" s="0"/>
@@ -6080,7 +6144,10 @@
       <c r="X141" s="0"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0"/>
+      <c r="A142" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B142" s="0"/>
       <c r="C142" s="0"/>
       <c r="D142" s="0"/>
       <c r="E142" s="0"/>
@@ -6104,7 +6171,10 @@
       <c r="X142" s="0"/>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0"/>
+      <c r="A143" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B143" s="0"/>
       <c r="C143" s="0"/>
       <c r="D143" s="0"/>
       <c r="E143" s="0"/>
@@ -6128,7 +6198,10 @@
       <c r="X143" s="0"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0"/>
+      <c r="A144" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B144" s="0"/>
       <c r="C144" s="0"/>
       <c r="D144" s="0"/>
       <c r="E144" s="0"/>
@@ -6151,71 +6224,34 @@
       <c r="W144" s="0"/>
       <c r="X144" s="0"/>
     </row>
-    <row r="145" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C145" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D145" s="2"/>
-      <c r="E145" s="2"/>
-      <c r="F145" s="2"/>
-      <c r="G145" s="2"/>
-      <c r="H145" s="2" t="n">
-        <v>5.65969879518072</v>
-      </c>
-      <c r="I145" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="J145" s="2" t="n">
-        <v>117</v>
-      </c>
-      <c r="K145" s="2" t="n">
-        <v>170.82</v>
-      </c>
-      <c r="L145" s="2" t="n">
-        <v>0.514518072289157</v>
-      </c>
-      <c r="M145" s="4" t="n">
-        <v>332</v>
-      </c>
-      <c r="N145" s="2" t="n">
-        <v>0.00909589041095891</v>
-      </c>
-      <c r="O145" s="2" t="n">
-        <v>0.227397260273973</v>
-      </c>
-      <c r="P145" s="2" t="n">
-        <v>30.1818181818182</v>
-      </c>
-      <c r="Q145" s="2" t="n">
-        <v>0.0826899128268991</v>
-      </c>
-      <c r="R145" s="2" t="n">
-        <v>0.90958904109589</v>
-      </c>
-      <c r="T145" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="U145" s="2" t="n">
-        <v>3.38</v>
-      </c>
-      <c r="V145" s="2" t="n">
-        <v>308.425</v>
-      </c>
-      <c r="W145" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="X145" s="2" t="n">
-        <v>3.38</v>
-      </c>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0"/>
+      <c r="B145" s="0"/>
+      <c r="C145" s="0"/>
+      <c r="D145" s="0"/>
+      <c r="E145" s="0"/>
+      <c r="F145" s="0"/>
+      <c r="G145" s="0"/>
+      <c r="H145" s="0"/>
+      <c r="I145" s="0"/>
+      <c r="J145" s="0"/>
+      <c r="K145" s="0"/>
+      <c r="L145" s="0"/>
+      <c r="M145" s="0"/>
+      <c r="N145" s="0"/>
+      <c r="O145" s="0"/>
+      <c r="P145" s="0"/>
+      <c r="Q145" s="0"/>
+      <c r="R145" s="0"/>
+      <c r="T145" s="0"/>
+      <c r="U145" s="0"/>
+      <c r="V145" s="0"/>
+      <c r="W145" s="0"/>
+      <c r="X145" s="0"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0"/>
+      <c r="B146" s="0"/>
       <c r="C146" s="0"/>
       <c r="D146" s="0"/>
       <c r="E146" s="0"/>
@@ -6238,71 +6274,34 @@
       <c r="W146" s="0"/>
       <c r="X146" s="0"/>
     </row>
-    <row r="147" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C147" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="D147" s="2"/>
-      <c r="E147" s="2"/>
-      <c r="F147" s="2"/>
-      <c r="G147" s="2"/>
-      <c r="H147" s="2" t="n">
-        <v>3.20712430426716</v>
-      </c>
-      <c r="I147" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="J147" s="2" t="n">
-        <v>148</v>
-      </c>
-      <c r="K147" s="2" t="n">
-        <v>216.08</v>
-      </c>
-      <c r="L147" s="2" t="n">
-        <v>0.400890538033395</v>
-      </c>
-      <c r="M147" s="4" t="n">
-        <v>539</v>
-      </c>
-      <c r="N147" s="2" t="n">
-        <v>0.0147671232876712</v>
-      </c>
-      <c r="O147" s="2" t="n">
-        <v>0.369178082191781</v>
-      </c>
-      <c r="P147" s="2" t="n">
-        <v>67.375</v>
-      </c>
-      <c r="Q147" s="2" t="n">
-        <v>0.18458904109589</v>
-      </c>
-      <c r="R147" s="2" t="n">
-        <v>1.47671232876712</v>
-      </c>
-      <c r="T147" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="U147" s="2" t="n">
-        <v>3.82</v>
-      </c>
-      <c r="V147" s="2" t="n">
-        <v>348.575</v>
-      </c>
-      <c r="W147" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="X147" s="2" t="n">
-        <v>3.82</v>
-      </c>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0"/>
+      <c r="B147" s="0"/>
+      <c r="C147" s="0"/>
+      <c r="D147" s="0"/>
+      <c r="E147" s="0"/>
+      <c r="F147" s="0"/>
+      <c r="G147" s="0"/>
+      <c r="H147" s="0"/>
+      <c r="I147" s="0"/>
+      <c r="J147" s="0"/>
+      <c r="K147" s="0"/>
+      <c r="L147" s="0"/>
+      <c r="M147" s="0"/>
+      <c r="N147" s="0"/>
+      <c r="O147" s="0"/>
+      <c r="P147" s="0"/>
+      <c r="Q147" s="0"/>
+      <c r="R147" s="0"/>
+      <c r="T147" s="0"/>
+      <c r="U147" s="0"/>
+      <c r="V147" s="0"/>
+      <c r="W147" s="0"/>
+      <c r="X147" s="0"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0"/>
+      <c r="B148" s="0"/>
       <c r="C148" s="0"/>
       <c r="D148" s="0"/>
       <c r="E148" s="0"/>
@@ -6325,71 +6324,34 @@
       <c r="W148" s="0"/>
       <c r="X148" s="0"/>
     </row>
-    <row r="149" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C149" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D149" s="2"/>
-      <c r="E149" s="2"/>
-      <c r="F149" s="2"/>
-      <c r="G149" s="2"/>
-      <c r="H149" s="2" t="n">
-        <v>3.69359877488515</v>
-      </c>
-      <c r="I149" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="J149" s="2" t="n">
-        <v>236</v>
-      </c>
-      <c r="K149" s="2" t="n">
-        <v>344.56</v>
-      </c>
-      <c r="L149" s="2" t="n">
-        <v>0.527656967840735</v>
-      </c>
-      <c r="M149" s="4" t="n">
-        <v>653</v>
-      </c>
-      <c r="N149" s="2" t="n">
-        <v>0.0178904109589041</v>
-      </c>
-      <c r="O149" s="2" t="n">
-        <v>0.447260273972603</v>
-      </c>
-      <c r="P149" s="2" t="n">
-        <v>93.2857142857143</v>
-      </c>
-      <c r="Q149" s="2" t="n">
-        <v>0.255577299412916</v>
-      </c>
-      <c r="R149" s="2" t="n">
-        <v>1.78904109589041</v>
-      </c>
-      <c r="T149" s="2" t="n">
-        <v>22</v>
-      </c>
-      <c r="U149" s="2" t="n">
-        <v>4.26</v>
-      </c>
-      <c r="V149" s="2" t="n">
-        <v>388.725</v>
-      </c>
-      <c r="W149" s="2" t="n">
-        <v>22</v>
-      </c>
-      <c r="X149" s="2" t="n">
-        <v>4.26</v>
-      </c>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0"/>
+      <c r="B149" s="0"/>
+      <c r="C149" s="0"/>
+      <c r="D149" s="0"/>
+      <c r="E149" s="0"/>
+      <c r="F149" s="0"/>
+      <c r="G149" s="0"/>
+      <c r="H149" s="0"/>
+      <c r="I149" s="0"/>
+      <c r="J149" s="0"/>
+      <c r="K149" s="0"/>
+      <c r="L149" s="0"/>
+      <c r="M149" s="0"/>
+      <c r="N149" s="0"/>
+      <c r="O149" s="0"/>
+      <c r="P149" s="0"/>
+      <c r="Q149" s="0"/>
+      <c r="R149" s="0"/>
+      <c r="T149" s="0"/>
+      <c r="U149" s="0"/>
+      <c r="V149" s="0"/>
+      <c r="W149" s="0"/>
+      <c r="X149" s="0"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0"/>
+      <c r="B150" s="0"/>
       <c r="C150" s="0"/>
       <c r="D150" s="0"/>
       <c r="E150" s="0"/>
@@ -6414,156 +6376,158 @@
     </row>
     <row r="151" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C151" s="2" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
       <c r="H151" s="2" t="n">
-        <v>3.17172413793103</v>
+        <v>5.65969879518072</v>
       </c>
       <c r="I151" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J151" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="K151" s="2" t="n">
+        <v>170.82</v>
+      </c>
+      <c r="L151" s="2" t="n">
+        <v>0.514518072289157</v>
+      </c>
+      <c r="M151" s="4" t="n">
+        <v>332</v>
+      </c>
+      <c r="N151" s="2" t="n">
+        <v>0.00909589041095891</v>
+      </c>
+      <c r="O151" s="2" t="n">
+        <v>0.227397260273973</v>
+      </c>
+      <c r="P151" s="2" t="n">
+        <v>30.1818181818182</v>
+      </c>
+      <c r="Q151" s="2" t="n">
+        <v>0.0826899128268991</v>
+      </c>
+      <c r="R151" s="2" t="n">
+        <v>0.90958904109589</v>
+      </c>
+      <c r="T151" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="U151" s="2" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="V151" s="2" t="n">
+        <v>308.425</v>
+      </c>
+      <c r="W151" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="X151" s="2" t="n">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0"/>
+      <c r="B152" s="0"/>
+      <c r="C152" s="0"/>
+      <c r="D152" s="0"/>
+      <c r="E152" s="0"/>
+      <c r="F152" s="0"/>
+      <c r="G152" s="0"/>
+      <c r="H152" s="0"/>
+      <c r="I152" s="0"/>
+      <c r="J152" s="0"/>
+      <c r="K152" s="0"/>
+      <c r="L152" s="0"/>
+      <c r="M152" s="0"/>
+      <c r="N152" s="0"/>
+      <c r="O152" s="0"/>
+      <c r="P152" s="0"/>
+      <c r="Q152" s="0"/>
+      <c r="R152" s="0"/>
+      <c r="T152" s="0"/>
+      <c r="U152" s="0"/>
+      <c r="V152" s="0"/>
+      <c r="W152" s="0"/>
+      <c r="X152" s="0"/>
+    </row>
+    <row r="153" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C153" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D153" s="2"/>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="2"/>
+      <c r="H153" s="2" t="n">
+        <v>3.20712430426716</v>
+      </c>
+      <c r="I153" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="J151" s="2" t="n">
-        <v>99</v>
-      </c>
-      <c r="K151" s="2" t="n">
-        <v>144.54</v>
-      </c>
-      <c r="L151" s="2" t="n">
-        <v>0.453103448275862</v>
-      </c>
-      <c r="M151" s="4" t="n">
-        <v>319</v>
-      </c>
-      <c r="N151" s="2" t="n">
-        <v>0.00873972602739726</v>
-      </c>
-      <c r="O151" s="2" t="n">
-        <v>0.218493150684931</v>
-      </c>
-      <c r="P151" s="2" t="n">
-        <v>45.5714285714286</v>
-      </c>
-      <c r="Q151" s="2" t="n">
-        <v>0.124853228962818</v>
-      </c>
-      <c r="R151" s="2" t="n">
-        <v>0.873972602739726</v>
-      </c>
-      <c r="T151" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="U151" s="2" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="V151" s="2" t="n">
-        <v>428.875</v>
-      </c>
-      <c r="W151" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="X151" s="2" t="n">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C152" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D152" s="2"/>
-      <c r="E152" s="2"/>
-      <c r="F152" s="2"/>
-      <c r="G152" s="2"/>
-      <c r="H152" s="2" t="n">
-        <v>2.65275908479139</v>
-      </c>
-      <c r="I152" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J152" s="2" t="n">
-        <v>225</v>
-      </c>
-      <c r="K152" s="2" t="n">
-        <v>328.5</v>
-      </c>
-      <c r="L152" s="2" t="n">
-        <v>0.442126514131898</v>
-      </c>
-      <c r="M152" s="2" t="n">
-        <v>743</v>
-      </c>
-      <c r="N152" s="2" t="n">
-        <v>0.0203561643835616</v>
-      </c>
-      <c r="O152" s="2" t="n">
-        <v>0.508904109589041</v>
-      </c>
-      <c r="P152" s="2" t="n">
-        <v>123.833333333333</v>
-      </c>
-      <c r="Q152" s="2" t="n">
-        <v>0.339269406392694</v>
-      </c>
-      <c r="R152" s="2" t="n">
-        <v>2.03561643835616</v>
-      </c>
-      <c r="T152" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="U152" s="2" t="n">
-        <v>4.92</v>
-      </c>
-      <c r="V152" s="2" t="n">
-        <v>448.95</v>
-      </c>
-      <c r="W152" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="X152" s="2" t="n">
-        <v>4.92</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0"/>
-      <c r="C153" s="0"/>
-      <c r="D153" s="0"/>
-      <c r="E153" s="0"/>
-      <c r="F153" s="0"/>
-      <c r="G153" s="0"/>
-      <c r="H153" s="0"/>
-      <c r="I153" s="0"/>
-      <c r="J153" s="0"/>
-      <c r="K153" s="0"/>
-      <c r="L153" s="0"/>
-      <c r="M153" s="0"/>
-      <c r="N153" s="0"/>
-      <c r="O153" s="0"/>
-      <c r="P153" s="0"/>
-      <c r="Q153" s="0"/>
-      <c r="R153" s="0"/>
-      <c r="T153" s="0"/>
-      <c r="U153" s="0"/>
-      <c r="V153" s="0"/>
-      <c r="W153" s="0"/>
-      <c r="X153" s="0"/>
+      <c r="J153" s="2" t="n">
+        <v>148</v>
+      </c>
+      <c r="K153" s="2" t="n">
+        <v>216.08</v>
+      </c>
+      <c r="L153" s="2" t="n">
+        <v>0.400890538033395</v>
+      </c>
+      <c r="M153" s="4" t="n">
+        <v>539</v>
+      </c>
+      <c r="N153" s="2" t="n">
+        <v>0.0147671232876712</v>
+      </c>
+      <c r="O153" s="2" t="n">
+        <v>0.369178082191781</v>
+      </c>
+      <c r="P153" s="2" t="n">
+        <v>67.375</v>
+      </c>
+      <c r="Q153" s="2" t="n">
+        <v>0.18458904109589</v>
+      </c>
+      <c r="R153" s="2" t="n">
+        <v>1.47671232876712</v>
+      </c>
+      <c r="T153" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U153" s="2" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="V153" s="2" t="n">
+        <v>348.575</v>
+      </c>
+      <c r="W153" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="X153" s="2" t="n">
+        <v>3.82</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0"/>
+      <c r="B154" s="0"/>
       <c r="C154" s="0"/>
       <c r="D154" s="0"/>
       <c r="E154" s="0"/>
@@ -6586,208 +6550,218 @@
       <c r="W154" s="0"/>
       <c r="X154" s="0"/>
     </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0"/>
-      <c r="C155" s="0"/>
-      <c r="D155" s="0"/>
-      <c r="E155" s="0"/>
-      <c r="F155" s="0"/>
-      <c r="G155" s="0"/>
-      <c r="H155" s="0"/>
-      <c r="I155" s="0"/>
-      <c r="J155" s="0"/>
-      <c r="K155" s="0"/>
-      <c r="L155" s="0"/>
-      <c r="M155" s="0"/>
-      <c r="N155" s="0"/>
-      <c r="O155" s="0"/>
-      <c r="P155" s="0"/>
-      <c r="Q155" s="0"/>
-      <c r="R155" s="0"/>
-      <c r="T155" s="0"/>
-      <c r="U155" s="0"/>
-      <c r="V155" s="0"/>
-      <c r="W155" s="0"/>
-      <c r="X155" s="0"/>
+    <row r="155" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C155" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D155" s="2"/>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+      <c r="H155" s="2" t="n">
+        <v>3.69359877488515</v>
+      </c>
+      <c r="I155" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J155" s="2" t="n">
+        <v>236</v>
+      </c>
+      <c r="K155" s="2" t="n">
+        <v>344.56</v>
+      </c>
+      <c r="L155" s="2" t="n">
+        <v>0.527656967840735</v>
+      </c>
+      <c r="M155" s="4" t="n">
+        <v>653</v>
+      </c>
+      <c r="N155" s="2" t="n">
+        <v>0.0178904109589041</v>
+      </c>
+      <c r="O155" s="2" t="n">
+        <v>0.447260273972603</v>
+      </c>
+      <c r="P155" s="2" t="n">
+        <v>93.2857142857143</v>
+      </c>
+      <c r="Q155" s="2" t="n">
+        <v>0.255577299412916</v>
+      </c>
+      <c r="R155" s="2" t="n">
+        <v>1.78904109589041</v>
+      </c>
+      <c r="T155" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="U155" s="2" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="V155" s="2" t="n">
+        <v>388.725</v>
+      </c>
+      <c r="W155" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="X155" s="2" t="n">
+        <v>4.26</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C156" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D156" s="2"/>
-      <c r="E156" s="2"/>
-      <c r="F156" s="2"/>
-      <c r="G156" s="2"/>
-      <c r="H156" s="2" t="n">
-        <v>1.2155023923445</v>
-      </c>
-      <c r="I156" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J156" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="K156" s="2" t="n">
-        <v>42.34</v>
-      </c>
-      <c r="L156" s="2" t="n">
-        <v>0.202583732057416</v>
-      </c>
-      <c r="M156" s="2" t="n">
-        <v>209</v>
-      </c>
-      <c r="N156" s="2" t="n">
-        <v>0.00572602739726027</v>
-      </c>
-      <c r="O156" s="2" t="n">
-        <v>0.143150684931507</v>
-      </c>
-      <c r="P156" s="2" t="n">
-        <v>34.8333333333333</v>
-      </c>
-      <c r="Q156" s="2" t="n">
-        <v>0.0954337899543379</v>
-      </c>
-      <c r="R156" s="2" t="n">
-        <v>0.572602739726027</v>
-      </c>
-      <c r="T156" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="U156" s="2" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="V156" s="2" t="n">
-        <v>529.25</v>
-      </c>
-      <c r="W156" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="X156" s="2" t="n">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0"/>
+      <c r="B156" s="0"/>
+      <c r="C156" s="0"/>
+      <c r="D156" s="0"/>
+      <c r="E156" s="0"/>
+      <c r="F156" s="0"/>
+      <c r="G156" s="0"/>
+      <c r="H156" s="0"/>
+      <c r="I156" s="0"/>
+      <c r="J156" s="0"/>
+      <c r="K156" s="0"/>
+      <c r="L156" s="0"/>
+      <c r="M156" s="0"/>
+      <c r="N156" s="0"/>
+      <c r="O156" s="0"/>
+      <c r="P156" s="0"/>
+      <c r="Q156" s="0"/>
+      <c r="R156" s="0"/>
+      <c r="T156" s="0"/>
+      <c r="U156" s="0"/>
+      <c r="V156" s="0"/>
+      <c r="W156" s="0"/>
+      <c r="X156" s="0"/>
+    </row>
+    <row r="157" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="C157" s="2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
       <c r="F157" s="2"/>
       <c r="G157" s="2"/>
       <c r="H157" s="2" t="n">
-        <v>1.6504347826087</v>
+        <v>3.17172413793103</v>
       </c>
       <c r="I157" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J157" s="2" t="n">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="K157" s="2" t="n">
-        <v>75.92</v>
+        <v>144.54</v>
       </c>
       <c r="L157" s="2" t="n">
-        <v>0.412608695652174</v>
-      </c>
-      <c r="M157" s="2" t="n">
-        <v>184</v>
+        <v>0.453103448275862</v>
+      </c>
+      <c r="M157" s="4" t="n">
+        <v>319</v>
       </c>
       <c r="N157" s="2" t="n">
-        <v>0.00504109589041096</v>
+        <v>0.00873972602739726</v>
       </c>
       <c r="O157" s="2" t="n">
-        <v>0.126027397260274</v>
+        <v>0.218493150684931</v>
       </c>
       <c r="P157" s="2" t="n">
-        <v>46</v>
+        <v>45.5714285714286</v>
       </c>
       <c r="Q157" s="2" t="n">
-        <v>0.126027397260274</v>
+        <v>0.124853228962818</v>
       </c>
       <c r="R157" s="2" t="n">
-        <v>0.504109589041096</v>
+        <v>0.873972602739726</v>
       </c>
       <c r="T157" s="2" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="U157" s="2" t="n">
-        <v>6.02</v>
+        <v>4.7</v>
       </c>
       <c r="V157" s="2" t="n">
-        <v>549.325</v>
+        <v>428.875</v>
       </c>
       <c r="W157" s="2" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="X157" s="2" t="n">
-        <v>6.02</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="C158" s="2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
       <c r="H158" s="2" t="n">
-        <v>1.21393258426966</v>
+        <v>2.65275908479139</v>
       </c>
       <c r="I158" s="2" t="n">
         <v>2</v>
       </c>
       <c r="J158" s="2" t="n">
-        <v>37</v>
+        <v>225</v>
       </c>
       <c r="K158" s="2" t="n">
-        <v>54.02</v>
+        <v>328.5</v>
       </c>
       <c r="L158" s="2" t="n">
-        <v>0.303483146067416</v>
-      </c>
-      <c r="M158" s="4" t="n">
-        <v>178</v>
+        <v>0.442126514131898</v>
+      </c>
+      <c r="M158" s="2" t="n">
+        <v>743</v>
       </c>
       <c r="N158" s="2" t="n">
-        <v>0.00487671232876712</v>
+        <v>0.0203561643835616</v>
       </c>
       <c r="O158" s="2" t="n">
-        <v>0.121917808219178</v>
+        <v>0.508904109589041</v>
       </c>
       <c r="P158" s="2" t="n">
-        <v>44.5</v>
+        <v>123.833333333333</v>
       </c>
       <c r="Q158" s="2" t="n">
-        <v>0.121917808219178</v>
+        <v>0.339269406392694</v>
       </c>
       <c r="R158" s="2" t="n">
-        <v>0.487671232876712</v>
+        <v>2.03561643835616</v>
       </c>
       <c r="T158" s="2" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="U158" s="2" t="n">
-        <v>6.24</v>
+        <v>4.92</v>
       </c>
       <c r="V158" s="2" t="n">
-        <v>569.4</v>
+        <v>448.95</v>
       </c>
       <c r="W158" s="2" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="X158" s="2" t="n">
-        <v>6.24</v>
+        <v>4.92</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6815,267 +6789,231 @@
       <c r="X159" s="0"/>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C160" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
-      <c r="G160" s="2"/>
-      <c r="H160" s="2" t="n">
-        <v>0.929090909090909</v>
-      </c>
-      <c r="I160" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J160" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="K160" s="2" t="n">
-        <v>30.66</v>
-      </c>
-      <c r="L160" s="2" t="n">
-        <v>0.30969696969697</v>
-      </c>
-      <c r="M160" s="2" t="n">
-        <v>99</v>
-      </c>
-      <c r="N160" s="2" t="n">
-        <v>0.00271232876712329</v>
-      </c>
-      <c r="O160" s="2" t="n">
-        <v>0.0678082191780822</v>
-      </c>
-      <c r="P160" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="Q160" s="2" t="n">
-        <v>0.0904109589041096</v>
-      </c>
-      <c r="R160" s="2" t="n">
-        <v>0.271232876712329</v>
-      </c>
-      <c r="T160" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="U160" s="2" t="n">
-        <v>6.68</v>
-      </c>
-      <c r="V160" s="2" t="n">
-        <v>609.55</v>
-      </c>
-      <c r="W160" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="X160" s="2" t="n">
-        <v>6.68</v>
-      </c>
+      <c r="A160" s="0"/>
+      <c r="C160" s="0"/>
+      <c r="D160" s="0"/>
+      <c r="E160" s="0"/>
+      <c r="F160" s="0"/>
+      <c r="G160" s="0"/>
+      <c r="H160" s="0"/>
+      <c r="I160" s="0"/>
+      <c r="J160" s="0"/>
+      <c r="K160" s="0"/>
+      <c r="L160" s="0"/>
+      <c r="M160" s="0"/>
+      <c r="N160" s="0"/>
+      <c r="O160" s="0"/>
+      <c r="P160" s="0"/>
+      <c r="Q160" s="0"/>
+      <c r="R160" s="0"/>
+      <c r="T160" s="0"/>
+      <c r="U160" s="0"/>
+      <c r="V160" s="0"/>
+      <c r="W160" s="0"/>
+      <c r="X160" s="0"/>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C161" s="2" t="n">
+      <c r="A161" s="0"/>
+      <c r="C161" s="0"/>
+      <c r="D161" s="0"/>
+      <c r="E161" s="0"/>
+      <c r="F161" s="0"/>
+      <c r="G161" s="0"/>
+      <c r="H161" s="0"/>
+      <c r="I161" s="0"/>
+      <c r="J161" s="0"/>
+      <c r="K161" s="0"/>
+      <c r="L161" s="0"/>
+      <c r="M161" s="0"/>
+      <c r="N161" s="0"/>
+      <c r="O161" s="0"/>
+      <c r="P161" s="0"/>
+      <c r="Q161" s="0"/>
+      <c r="R161" s="0"/>
+      <c r="T161" s="0"/>
+      <c r="U161" s="0"/>
+      <c r="V161" s="0"/>
+      <c r="W161" s="0"/>
+      <c r="X161" s="0"/>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C162" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D162" s="2"/>
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="2"/>
+      <c r="H162" s="2" t="n">
+        <v>1.2155023923445</v>
+      </c>
+      <c r="I162" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D161" s="2"/>
-      <c r="E161" s="2"/>
-      <c r="F161" s="2"/>
-      <c r="G161" s="2"/>
-      <c r="H161" s="2" t="n">
-        <v>0.925853658536585</v>
-      </c>
-      <c r="I161" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J161" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="K161" s="2" t="n">
-        <v>18.98</v>
-      </c>
-      <c r="L161" s="2" t="n">
-        <v>0.462926829268293</v>
-      </c>
-      <c r="M161" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="N161" s="2" t="n">
-        <v>0.00112328767123288</v>
-      </c>
-      <c r="O161" s="2" t="n">
-        <v>0.0280821917808219</v>
-      </c>
-      <c r="P161" s="2" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="Q161" s="2" t="n">
-        <v>0.0561643835616438</v>
-      </c>
-      <c r="R161" s="2" t="n">
-        <v>0.112328767123288</v>
-      </c>
-      <c r="T161" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="U161" s="2" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="V161" s="2" t="n">
-        <v>629.625</v>
-      </c>
-      <c r="W161" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="X161" s="2" t="n">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0"/>
-      <c r="C162" s="0"/>
-      <c r="D162" s="0"/>
-      <c r="E162" s="0"/>
-      <c r="F162" s="0"/>
-      <c r="G162" s="0"/>
-      <c r="H162" s="0"/>
-      <c r="I162" s="0"/>
-      <c r="J162" s="0"/>
-      <c r="K162" s="0"/>
-      <c r="L162" s="0"/>
-      <c r="M162" s="0"/>
-      <c r="N162" s="0"/>
-      <c r="O162" s="0"/>
-      <c r="P162" s="0"/>
-      <c r="Q162" s="0"/>
-      <c r="R162" s="0"/>
-      <c r="T162" s="0"/>
-      <c r="U162" s="0"/>
-      <c r="V162" s="0"/>
-      <c r="W162" s="0"/>
-      <c r="X162" s="0"/>
+      <c r="J162" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="K162" s="2" t="n">
+        <v>42.34</v>
+      </c>
+      <c r="L162" s="2" t="n">
+        <v>0.202583732057416</v>
+      </c>
+      <c r="M162" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="N162" s="2" t="n">
+        <v>0.00572602739726027</v>
+      </c>
+      <c r="O162" s="2" t="n">
+        <v>0.143150684931507</v>
+      </c>
+      <c r="P162" s="2" t="n">
+        <v>34.8333333333333</v>
+      </c>
+      <c r="Q162" s="2" t="n">
+        <v>0.0954337899543379</v>
+      </c>
+      <c r="R162" s="2" t="n">
+        <v>0.572602739726027</v>
+      </c>
+      <c r="T162" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="U162" s="2" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="V162" s="2" t="n">
+        <v>529.25</v>
+      </c>
+      <c r="W162" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="X162" s="2" t="n">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C163" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
       <c r="H163" s="2" t="n">
-        <v>1.21666666666667</v>
+        <v>1.6504347826087</v>
       </c>
       <c r="I163" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J163" s="2" t="n">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="K163" s="2" t="n">
-        <v>36.5</v>
+        <v>75.92</v>
       </c>
       <c r="L163" s="2" t="n">
-        <v>1.21666666666667</v>
+        <v>0.412608695652174</v>
       </c>
       <c r="M163" s="2" t="n">
+        <v>184</v>
+      </c>
+      <c r="N163" s="2" t="n">
+        <v>0.00504109589041096</v>
+      </c>
+      <c r="O163" s="2" t="n">
+        <v>0.126027397260274</v>
+      </c>
+      <c r="P163" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q163" s="2" t="n">
+        <v>0.126027397260274</v>
+      </c>
+      <c r="R163" s="2" t="n">
+        <v>0.504109589041096</v>
+      </c>
+      <c r="T163" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="N163" s="2" t="n">
-        <v>0.000821917808219178</v>
-      </c>
-      <c r="O163" s="2" t="n">
-        <v>0.0205479452054794</v>
-      </c>
-      <c r="P163" s="2" t="n">
+      <c r="U163" s="2" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="V163" s="2" t="n">
+        <v>549.325</v>
+      </c>
+      <c r="W163" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="Q163" s="2" t="n">
-        <v>0.0821917808219178</v>
-      </c>
-      <c r="R163" s="2" t="n">
-        <v>0.0821917808219178</v>
-      </c>
-      <c r="T163" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="U163" s="2" t="n">
-        <v>7.34</v>
-      </c>
-      <c r="V163" s="2" t="n">
-        <v>669.775</v>
-      </c>
-      <c r="W163" s="2" t="n">
-        <v>36</v>
-      </c>
       <c r="X163" s="2" t="n">
-        <v>7.34</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.02</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C164" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
       <c r="H164" s="2" t="n">
-        <v>0.297959183673469</v>
+        <v>1.21393258426966</v>
       </c>
       <c r="I164" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J164" s="2" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="K164" s="2" t="n">
-        <v>14.6</v>
+        <v>54.02</v>
       </c>
       <c r="L164" s="2" t="n">
-        <v>0.297959183673469</v>
-      </c>
-      <c r="M164" s="2" t="n">
-        <v>49</v>
+        <v>0.303483146067416</v>
+      </c>
+      <c r="M164" s="4" t="n">
+        <v>178</v>
       </c>
       <c r="N164" s="2" t="n">
-        <v>0.00134246575342466</v>
+        <v>0.00487671232876712</v>
       </c>
       <c r="O164" s="2" t="n">
-        <v>0.0335616438356164</v>
+        <v>0.121917808219178</v>
       </c>
       <c r="P164" s="2" t="n">
-        <v>49</v>
+        <v>44.5</v>
       </c>
       <c r="Q164" s="2" t="n">
-        <v>0.134246575342466</v>
+        <v>0.121917808219178</v>
       </c>
       <c r="R164" s="2" t="n">
-        <v>0.134246575342466</v>
+        <v>0.487671232876712</v>
       </c>
       <c r="T164" s="2" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="U164" s="2" t="n">
-        <v>7.56</v>
+        <v>6.24</v>
       </c>
       <c r="V164" s="2" t="n">
-        <v>689.85</v>
+        <v>569.4</v>
       </c>
       <c r="W164" s="2" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="X164" s="2" t="n">
-        <v>7.56</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7085,75 +7023,141 @@
       <c r="E165" s="0"/>
       <c r="F165" s="0"/>
       <c r="G165" s="0"/>
+      <c r="H165" s="0"/>
+      <c r="I165" s="0"/>
       <c r="J165" s="0"/>
       <c r="K165" s="0"/>
+      <c r="L165" s="0"/>
       <c r="M165" s="0"/>
-      <c r="T165" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="U165" s="2" t="n">
-        <v>7.78</v>
-      </c>
-      <c r="V165" s="2" t="n">
-        <v>709.925</v>
-      </c>
-      <c r="W165" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="X165" s="2" t="n">
-        <v>7.78</v>
-      </c>
+      <c r="N165" s="0"/>
+      <c r="O165" s="0"/>
+      <c r="P165" s="0"/>
+      <c r="Q165" s="0"/>
+      <c r="R165" s="0"/>
+      <c r="T165" s="0"/>
+      <c r="U165" s="0"/>
+      <c r="V165" s="0"/>
+      <c r="W165" s="0"/>
+      <c r="X165" s="0"/>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0"/>
-      <c r="C166" s="0"/>
-      <c r="D166" s="0"/>
-      <c r="E166" s="0"/>
-      <c r="F166" s="0"/>
-      <c r="G166" s="0"/>
-      <c r="J166" s="0"/>
-      <c r="K166" s="0"/>
-      <c r="M166" s="0"/>
+      <c r="A166" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C166" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D166" s="2"/>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+      <c r="H166" s="2" t="n">
+        <v>0.929090909090909</v>
+      </c>
+      <c r="I166" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J166" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K166" s="2" t="n">
+        <v>30.66</v>
+      </c>
+      <c r="L166" s="2" t="n">
+        <v>0.30969696969697</v>
+      </c>
+      <c r="M166" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="N166" s="2" t="n">
+        <v>0.00271232876712329</v>
+      </c>
+      <c r="O166" s="2" t="n">
+        <v>0.0678082191780822</v>
+      </c>
+      <c r="P166" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q166" s="2" t="n">
+        <v>0.0904109589041096</v>
+      </c>
+      <c r="R166" s="2" t="n">
+        <v>0.271232876712329</v>
+      </c>
       <c r="T166" s="2" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="U166" s="2" t="n">
-        <v>8</v>
+        <v>6.68</v>
       </c>
       <c r="V166" s="2" t="n">
-        <v>730</v>
+        <v>609.55</v>
       </c>
       <c r="W166" s="2" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="X166" s="2" t="n">
-        <v>8</v>
+        <v>6.68</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0"/>
-      <c r="C167" s="0"/>
-      <c r="D167" s="0"/>
-      <c r="E167" s="0"/>
-      <c r="F167" s="0"/>
-      <c r="G167" s="0"/>
-      <c r="J167" s="0"/>
-      <c r="K167" s="0"/>
-      <c r="M167" s="0"/>
+      <c r="A167" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C167" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D167" s="2"/>
+      <c r="E167" s="2"/>
+      <c r="F167" s="2"/>
+      <c r="G167" s="2"/>
+      <c r="H167" s="2" t="n">
+        <v>0.925853658536585</v>
+      </c>
+      <c r="I167" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J167" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="K167" s="2" t="n">
+        <v>18.98</v>
+      </c>
+      <c r="L167" s="2" t="n">
+        <v>0.462926829268293</v>
+      </c>
+      <c r="M167" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="N167" s="2" t="n">
+        <v>0.00112328767123288</v>
+      </c>
+      <c r="O167" s="2" t="n">
+        <v>0.0280821917808219</v>
+      </c>
+      <c r="P167" s="2" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="Q167" s="2" t="n">
+        <v>0.0561643835616438</v>
+      </c>
+      <c r="R167" s="2" t="n">
+        <v>0.112328767123288</v>
+      </c>
       <c r="T167" s="2" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="U167" s="2" t="n">
-        <v>8.22</v>
+        <v>6.9</v>
       </c>
       <c r="V167" s="2" t="n">
-        <v>750.075</v>
+        <v>629.625</v>
       </c>
       <c r="W167" s="2" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="X167" s="2" t="n">
-        <v>8.22</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7163,75 +7167,141 @@
       <c r="E168" s="0"/>
       <c r="F168" s="0"/>
       <c r="G168" s="0"/>
+      <c r="H168" s="0"/>
+      <c r="I168" s="0"/>
       <c r="J168" s="0"/>
       <c r="K168" s="0"/>
+      <c r="L168" s="0"/>
       <c r="M168" s="0"/>
-      <c r="T168" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="U168" s="2" t="n">
-        <v>9.32</v>
-      </c>
-      <c r="V168" s="2" t="n">
-        <v>850.45</v>
-      </c>
-      <c r="W168" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="X168" s="2" t="n">
-        <v>8.44</v>
-      </c>
+      <c r="N168" s="0"/>
+      <c r="O168" s="0"/>
+      <c r="P168" s="0"/>
+      <c r="Q168" s="0"/>
+      <c r="R168" s="0"/>
+      <c r="T168" s="0"/>
+      <c r="U168" s="0"/>
+      <c r="V168" s="0"/>
+      <c r="W168" s="0"/>
+      <c r="X168" s="0"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0"/>
-      <c r="C169" s="0"/>
-      <c r="D169" s="0"/>
-      <c r="E169" s="0"/>
-      <c r="F169" s="0"/>
-      <c r="G169" s="0"/>
-      <c r="J169" s="0"/>
-      <c r="K169" s="0"/>
-      <c r="M169" s="0"/>
+      <c r="A169" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C169" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D169" s="2"/>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="2"/>
+      <c r="H169" s="2" t="n">
+        <v>1.21666666666667</v>
+      </c>
+      <c r="I169" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J169" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="K169" s="2" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="L169" s="2" t="n">
+        <v>1.21666666666667</v>
+      </c>
+      <c r="M169" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="N169" s="2" t="n">
+        <v>0.000821917808219178</v>
+      </c>
+      <c r="O169" s="2" t="n">
+        <v>0.0205479452054794</v>
+      </c>
+      <c r="P169" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q169" s="2" t="n">
+        <v>0.0821917808219178</v>
+      </c>
+      <c r="R169" s="2" t="n">
+        <v>0.0821917808219178</v>
+      </c>
       <c r="T169" s="2" t="n">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="U169" s="2" t="n">
-        <v>10.42</v>
+        <v>7.34</v>
       </c>
       <c r="V169" s="2" t="n">
-        <v>950.825</v>
+        <v>669.775</v>
       </c>
       <c r="W169" s="2" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="X169" s="2" t="n">
-        <v>8.66</v>
+        <v>7.34</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="0"/>
-      <c r="C170" s="0"/>
-      <c r="D170" s="0"/>
-      <c r="E170" s="0"/>
-      <c r="F170" s="0"/>
-      <c r="G170" s="0"/>
-      <c r="J170" s="0"/>
-      <c r="K170" s="0"/>
-      <c r="M170" s="0"/>
+      <c r="A170" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C170" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D170" s="2"/>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="2"/>
+      <c r="H170" s="2" t="n">
+        <v>0.297959183673469</v>
+      </c>
+      <c r="I170" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J170" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="K170" s="2" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="L170" s="2" t="n">
+        <v>0.297959183673469</v>
+      </c>
+      <c r="M170" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="N170" s="2" t="n">
+        <v>0.00134246575342466</v>
+      </c>
+      <c r="O170" s="2" t="n">
+        <v>0.0335616438356164</v>
+      </c>
+      <c r="P170" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="Q170" s="2" t="n">
+        <v>0.134246575342466</v>
+      </c>
+      <c r="R170" s="2" t="n">
+        <v>0.134246575342466</v>
+      </c>
       <c r="T170" s="2" t="n">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="U170" s="2" t="n">
-        <v>11.52</v>
+        <v>7.56</v>
       </c>
       <c r="V170" s="2" t="n">
-        <v>1051.2</v>
+        <v>689.85</v>
       </c>
       <c r="W170" s="2" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="X170" s="2" t="n">
-        <v>8.88</v>
+        <v>7.56</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7245,19 +7315,19 @@
       <c r="K171" s="0"/>
       <c r="M171" s="0"/>
       <c r="T171" s="2" t="n">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="U171" s="2" t="n">
-        <v>12.62</v>
+        <v>7.78</v>
       </c>
       <c r="V171" s="2" t="n">
-        <v>1151.575</v>
+        <v>709.925</v>
       </c>
       <c r="W171" s="2" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="X171" s="2" t="n">
-        <v>9.1</v>
+        <v>7.78</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7271,19 +7341,19 @@
       <c r="K172" s="0"/>
       <c r="M172" s="0"/>
       <c r="T172" s="2" t="n">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="U172" s="2" t="n">
-        <v>13.72</v>
+        <v>8</v>
       </c>
       <c r="V172" s="2" t="n">
-        <v>1251.95</v>
+        <v>730</v>
       </c>
       <c r="W172" s="2" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="X172" s="2" t="n">
-        <v>9.32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7297,19 +7367,19 @@
       <c r="K173" s="0"/>
       <c r="M173" s="0"/>
       <c r="T173" s="2" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="U173" s="2" t="n">
-        <v>14.82</v>
+        <v>8.22</v>
       </c>
       <c r="V173" s="2" t="n">
-        <v>1352.325</v>
+        <v>750.075</v>
       </c>
       <c r="W173" s="2" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="X173" s="2" t="n">
-        <v>9.54</v>
+        <v>8.22</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7323,19 +7393,19 @@
       <c r="K174" s="0"/>
       <c r="M174" s="0"/>
       <c r="T174" s="2" t="n">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="U174" s="2" t="n">
-        <v>15.92</v>
+        <v>9.32</v>
       </c>
       <c r="V174" s="2" t="n">
-        <v>1452.7</v>
+        <v>850.45</v>
       </c>
       <c r="W174" s="2" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="X174" s="2" t="n">
-        <v>9.76</v>
+        <v>8.44</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7349,19 +7419,19 @@
       <c r="K175" s="0"/>
       <c r="M175" s="0"/>
       <c r="T175" s="2" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="U175" s="2" t="n">
-        <v>17.02</v>
+        <v>10.42</v>
       </c>
       <c r="V175" s="2" t="n">
-        <v>1553.075</v>
+        <v>950.825</v>
       </c>
       <c r="W175" s="2" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="X175" s="2" t="n">
-        <v>9.98</v>
+        <v>8.66</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7375,25 +7445,23 @@
       <c r="K176" s="0"/>
       <c r="M176" s="0"/>
       <c r="T176" s="2" t="n">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="U176" s="2" t="n">
-        <v>18.12</v>
+        <v>11.52</v>
       </c>
       <c r="V176" s="2" t="n">
-        <v>1653.45</v>
+        <v>1051.2</v>
       </c>
       <c r="W176" s="2" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="X176" s="2" t="n">
-        <v>10.2</v>
+        <v>8.88</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="A177" s="0"/>
       <c r="C177" s="0"/>
       <c r="D177" s="0"/>
       <c r="E177" s="0"/>
@@ -7403,25 +7471,23 @@
       <c r="K177" s="0"/>
       <c r="M177" s="0"/>
       <c r="T177" s="2" t="n">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="U177" s="2" t="n">
-        <v>20.32</v>
+        <v>12.62</v>
       </c>
       <c r="V177" s="2" t="n">
-        <v>1854.2</v>
+        <v>1151.575</v>
       </c>
       <c r="W177" s="2" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="X177" s="2" t="n">
-        <v>10.42</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="2" t="s">
-        <v>162</v>
-      </c>
+      <c r="A178" s="0"/>
       <c r="C178" s="0"/>
       <c r="D178" s="0"/>
       <c r="E178" s="0"/>
@@ -7431,19 +7497,19 @@
       <c r="K178" s="0"/>
       <c r="M178" s="0"/>
       <c r="T178" s="2" t="n">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="U178" s="2" t="n">
-        <v>22.52</v>
+        <v>13.72</v>
       </c>
       <c r="V178" s="2" t="n">
-        <v>2054.95</v>
+        <v>1251.95</v>
       </c>
       <c r="W178" s="2" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="X178" s="2" t="n">
-        <v>10.64</v>
+        <v>9.32</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7457,19 +7523,19 @@
       <c r="K179" s="0"/>
       <c r="M179" s="0"/>
       <c r="T179" s="2" t="n">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="U179" s="2" t="n">
-        <v>24.72</v>
+        <v>14.82</v>
       </c>
       <c r="V179" s="2" t="n">
-        <v>2255.7</v>
+        <v>1352.325</v>
       </c>
       <c r="W179" s="2" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="X179" s="2" t="n">
-        <v>10.86</v>
+        <v>9.54</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7483,19 +7549,19 @@
       <c r="K180" s="0"/>
       <c r="M180" s="0"/>
       <c r="T180" s="2" t="n">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="U180" s="2" t="n">
-        <v>26.92</v>
+        <v>15.92</v>
       </c>
       <c r="V180" s="2" t="n">
-        <v>2456.45</v>
+        <v>1452.7</v>
       </c>
       <c r="W180" s="2" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="X180" s="2" t="n">
-        <v>11.08</v>
+        <v>9.76</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7509,19 +7575,19 @@
       <c r="K181" s="0"/>
       <c r="M181" s="0"/>
       <c r="T181" s="2" t="n">
-        <v>135</v>
+        <v>80</v>
       </c>
       <c r="U181" s="2" t="n">
-        <v>29.12</v>
+        <v>17.02</v>
       </c>
       <c r="V181" s="2" t="n">
-        <v>2657.2</v>
+        <v>1553.075</v>
       </c>
       <c r="W181" s="2" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="X181" s="2" t="n">
-        <v>11.3</v>
+        <v>9.98</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7535,23 +7601,25 @@
       <c r="K182" s="0"/>
       <c r="M182" s="0"/>
       <c r="T182" s="2" t="n">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="U182" s="2" t="n">
-        <v>31.3199999999999</v>
+        <v>18.12</v>
       </c>
       <c r="V182" s="2" t="n">
-        <v>2857.94999999999</v>
+        <v>1653.45</v>
       </c>
       <c r="W182" s="2" t="n">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="X182" s="2" t="n">
-        <v>11.52</v>
+        <v>10.2</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0"/>
+      <c r="A183" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="C183" s="0"/>
       <c r="D183" s="0"/>
       <c r="E183" s="0"/>
@@ -7561,23 +7629,25 @@
       <c r="K183" s="0"/>
       <c r="M183" s="0"/>
       <c r="T183" s="2" t="n">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="U183" s="2" t="n">
-        <v>33.5199999999999</v>
+        <v>20.32</v>
       </c>
       <c r="V183" s="2" t="n">
-        <v>3058.69999999999</v>
+        <v>1854.2</v>
       </c>
       <c r="W183" s="2" t="n">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="X183" s="2" t="n">
-        <v>11.74</v>
+        <v>10.42</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0"/>
+      <c r="A184" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="C184" s="0"/>
       <c r="D184" s="0"/>
       <c r="E184" s="0"/>
@@ -7587,19 +7657,19 @@
       <c r="K184" s="0"/>
       <c r="M184" s="0"/>
       <c r="T184" s="2" t="n">
-        <v>165</v>
+        <v>105</v>
       </c>
       <c r="U184" s="2" t="n">
-        <v>35.7199999999999</v>
+        <v>22.52</v>
       </c>
       <c r="V184" s="2" t="n">
-        <v>3259.44999999999</v>
+        <v>2054.95</v>
       </c>
       <c r="W184" s="2" t="n">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="X184" s="2" t="n">
-        <v>11.96</v>
+        <v>10.64</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7613,19 +7683,19 @@
       <c r="K185" s="0"/>
       <c r="M185" s="0"/>
       <c r="T185" s="2" t="n">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="U185" s="2" t="n">
-        <v>37.9199999999999</v>
+        <v>24.72</v>
       </c>
       <c r="V185" s="2" t="n">
-        <v>3460.19999999999</v>
+        <v>2255.7</v>
       </c>
       <c r="W185" s="2" t="n">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="X185" s="2" t="n">
-        <v>12.18</v>
+        <v>10.86</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7639,19 +7709,19 @@
       <c r="K186" s="0"/>
       <c r="M186" s="0"/>
       <c r="T186" s="2" t="n">
-        <v>185</v>
+        <v>125</v>
       </c>
       <c r="U186" s="2" t="n">
-        <v>40.1199999999999</v>
+        <v>26.92</v>
       </c>
       <c r="V186" s="2" t="n">
-        <v>3660.94999999999</v>
+        <v>2456.45</v>
       </c>
       <c r="W186" s="2" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="X186" s="2" t="n">
-        <v>12.4</v>
+        <v>11.08</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7665,19 +7735,19 @@
       <c r="K187" s="0"/>
       <c r="M187" s="0"/>
       <c r="T187" s="2" t="n">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="U187" s="2" t="n">
-        <v>42.3199999999999</v>
+        <v>29.12</v>
       </c>
       <c r="V187" s="2" t="n">
-        <v>3861.69999999999</v>
+        <v>2657.2</v>
       </c>
       <c r="W187" s="2" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="X187" s="2" t="n">
-        <v>12.62</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7691,19 +7761,19 @@
       <c r="K188" s="0"/>
       <c r="M188" s="0"/>
       <c r="T188" s="2" t="n">
-        <v>205</v>
+        <v>145</v>
       </c>
       <c r="U188" s="2" t="n">
-        <v>44.5199999999999</v>
+        <v>31.3199999999999</v>
       </c>
       <c r="V188" s="2" t="n">
-        <v>4062.44999999999</v>
+        <v>2857.94999999999</v>
       </c>
       <c r="W188" s="2" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="X188" s="2" t="n">
-        <v>12.84</v>
+        <v>11.52</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7716,11 +7786,20 @@
       <c r="J189" s="0"/>
       <c r="K189" s="0"/>
       <c r="M189" s="0"/>
+      <c r="T189" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="U189" s="2" t="n">
+        <v>33.5199999999999</v>
+      </c>
+      <c r="V189" s="2" t="n">
+        <v>3058.69999999999</v>
+      </c>
       <c r="W189" s="2" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="X189" s="2" t="n">
-        <v>13.06</v>
+        <v>11.74</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7733,11 +7812,20 @@
       <c r="J190" s="0"/>
       <c r="K190" s="0"/>
       <c r="M190" s="0"/>
+      <c r="T190" s="2" t="n">
+        <v>165</v>
+      </c>
+      <c r="U190" s="2" t="n">
+        <v>35.7199999999999</v>
+      </c>
+      <c r="V190" s="2" t="n">
+        <v>3259.44999999999</v>
+      </c>
       <c r="W190" s="2" t="n">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="X190" s="2" t="n">
-        <v>13.28</v>
+        <v>11.96</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7750,11 +7838,20 @@
       <c r="J191" s="0"/>
       <c r="K191" s="0"/>
       <c r="M191" s="0"/>
+      <c r="T191" s="2" t="n">
+        <v>175</v>
+      </c>
+      <c r="U191" s="2" t="n">
+        <v>37.9199999999999</v>
+      </c>
+      <c r="V191" s="2" t="n">
+        <v>3460.19999999999</v>
+      </c>
       <c r="W191" s="2" t="n">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="X191" s="2" t="n">
-        <v>13.5</v>
+        <v>12.18</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7767,11 +7864,20 @@
       <c r="J192" s="0"/>
       <c r="K192" s="0"/>
       <c r="M192" s="0"/>
+      <c r="T192" s="2" t="n">
+        <v>185</v>
+      </c>
+      <c r="U192" s="2" t="n">
+        <v>40.1199999999999</v>
+      </c>
+      <c r="V192" s="2" t="n">
+        <v>3660.94999999999</v>
+      </c>
       <c r="W192" s="2" t="n">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="X192" s="2" t="n">
-        <v>13.72</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7784,11 +7890,20 @@
       <c r="J193" s="0"/>
       <c r="K193" s="0"/>
       <c r="M193" s="0"/>
+      <c r="T193" s="2" t="n">
+        <v>195</v>
+      </c>
+      <c r="U193" s="2" t="n">
+        <v>42.3199999999999</v>
+      </c>
+      <c r="V193" s="2" t="n">
+        <v>3861.69999999999</v>
+      </c>
       <c r="W193" s="2" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="X193" s="2" t="n">
-        <v>13.94</v>
+        <v>12.62</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7801,11 +7916,20 @@
       <c r="J194" s="0"/>
       <c r="K194" s="0"/>
       <c r="M194" s="0"/>
+      <c r="T194" s="2" t="n">
+        <v>205</v>
+      </c>
+      <c r="U194" s="2" t="n">
+        <v>44.5199999999999</v>
+      </c>
+      <c r="V194" s="2" t="n">
+        <v>4062.44999999999</v>
+      </c>
       <c r="W194" s="2" t="n">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="X194" s="2" t="n">
-        <v>14.16</v>
+        <v>12.84</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7819,10 +7943,10 @@
       <c r="K195" s="0"/>
       <c r="M195" s="0"/>
       <c r="W195" s="2" t="n">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="X195" s="2" t="n">
-        <v>14.38</v>
+        <v>13.06</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7836,10 +7960,10 @@
       <c r="K196" s="0"/>
       <c r="M196" s="0"/>
       <c r="W196" s="2" t="n">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="X196" s="2" t="n">
-        <v>14.6</v>
+        <v>13.28</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7853,10 +7977,10 @@
       <c r="K197" s="0"/>
       <c r="M197" s="0"/>
       <c r="W197" s="2" t="n">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="X197" s="2" t="n">
-        <v>14.82</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7870,10 +7994,10 @@
       <c r="K198" s="0"/>
       <c r="M198" s="0"/>
       <c r="W198" s="2" t="n">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="X198" s="2" t="n">
-        <v>15.04</v>
+        <v>13.72</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7887,10 +8011,10 @@
       <c r="K199" s="0"/>
       <c r="M199" s="0"/>
       <c r="W199" s="2" t="n">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="X199" s="2" t="n">
-        <v>15.26</v>
+        <v>13.94</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7904,10 +8028,10 @@
       <c r="K200" s="0"/>
       <c r="M200" s="0"/>
       <c r="W200" s="2" t="n">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="X200" s="2" t="n">
-        <v>15.48</v>
+        <v>14.16</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7921,10 +8045,10 @@
       <c r="K201" s="0"/>
       <c r="M201" s="0"/>
       <c r="W201" s="2" t="n">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="X201" s="2" t="n">
-        <v>15.7</v>
+        <v>14.38</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7938,10 +8062,10 @@
       <c r="K202" s="0"/>
       <c r="M202" s="0"/>
       <c r="W202" s="2" t="n">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="X202" s="2" t="n">
-        <v>15.92</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7955,10 +8079,10 @@
       <c r="K203" s="0"/>
       <c r="M203" s="0"/>
       <c r="W203" s="2" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="X203" s="2" t="n">
-        <v>16.14</v>
+        <v>14.82</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7972,1305 +8096,1407 @@
       <c r="K204" s="0"/>
       <c r="M204" s="0"/>
       <c r="W204" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="X204" s="2" t="n">
+        <v>15.04</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0"/>
+      <c r="C205" s="0"/>
+      <c r="D205" s="0"/>
+      <c r="E205" s="0"/>
+      <c r="F205" s="0"/>
+      <c r="G205" s="0"/>
+      <c r="J205" s="0"/>
+      <c r="K205" s="0"/>
+      <c r="M205" s="0"/>
+      <c r="W205" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="X205" s="2" t="n">
+        <v>15.26</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0"/>
+      <c r="C206" s="0"/>
+      <c r="D206" s="0"/>
+      <c r="E206" s="0"/>
+      <c r="F206" s="0"/>
+      <c r="G206" s="0"/>
+      <c r="J206" s="0"/>
+      <c r="K206" s="0"/>
+      <c r="M206" s="0"/>
+      <c r="W206" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="X206" s="2" t="n">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0"/>
+      <c r="C207" s="0"/>
+      <c r="D207" s="0"/>
+      <c r="E207" s="0"/>
+      <c r="F207" s="0"/>
+      <c r="G207" s="0"/>
+      <c r="J207" s="0"/>
+      <c r="K207" s="0"/>
+      <c r="M207" s="0"/>
+      <c r="W207" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="X207" s="2" t="n">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0"/>
+      <c r="C208" s="0"/>
+      <c r="D208" s="0"/>
+      <c r="E208" s="0"/>
+      <c r="F208" s="0"/>
+      <c r="G208" s="0"/>
+      <c r="J208" s="0"/>
+      <c r="K208" s="0"/>
+      <c r="M208" s="0"/>
+      <c r="W208" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="X208" s="2" t="n">
+        <v>15.92</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0"/>
+      <c r="C209" s="0"/>
+      <c r="D209" s="0"/>
+      <c r="E209" s="0"/>
+      <c r="F209" s="0"/>
+      <c r="G209" s="0"/>
+      <c r="J209" s="0"/>
+      <c r="K209" s="0"/>
+      <c r="M209" s="0"/>
+      <c r="W209" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="X209" s="2" t="n">
+        <v>16.14</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0"/>
+      <c r="C210" s="0"/>
+      <c r="D210" s="0"/>
+      <c r="E210" s="0"/>
+      <c r="F210" s="0"/>
+      <c r="G210" s="0"/>
+      <c r="J210" s="0"/>
+      <c r="K210" s="0"/>
+      <c r="M210" s="0"/>
+      <c r="W210" s="2" t="n">
         <v>77</v>
       </c>
-      <c r="X204" s="2" t="n">
+      <c r="X210" s="2" t="n">
         <v>16.36</v>
-      </c>
-    </row>
-    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D205" s="2"/>
-      <c r="E205" s="2"/>
-      <c r="F205" s="2"/>
-      <c r="G205" s="2"/>
-      <c r="J205" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="K205" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="M205" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="W205" s="2" t="n">
-        <v>78</v>
-      </c>
-      <c r="X205" s="2" t="n">
-        <v>16.58</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C206" s="2" t="n">
-        <v>98</v>
-      </c>
-      <c r="D206" s="2"/>
-      <c r="E206" s="2"/>
-      <c r="F206" s="2"/>
-      <c r="G206" s="2"/>
-      <c r="W206" s="2" t="n">
-        <v>79</v>
-      </c>
-      <c r="X206" s="2" t="n">
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C207" s="2" t="n">
-        <v>52</v>
-      </c>
-      <c r="D207" s="2"/>
-      <c r="E207" s="2"/>
-      <c r="F207" s="2"/>
-      <c r="G207" s="2"/>
-      <c r="W207" s="2" t="n">
-        <v>80</v>
-      </c>
-      <c r="X207" s="2" t="n">
-        <v>17.02</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C208" s="2" t="n">
-        <v>51</v>
-      </c>
-      <c r="D208" s="2"/>
-      <c r="E208" s="2"/>
-      <c r="F208" s="2"/>
-      <c r="G208" s="2"/>
-      <c r="W208" s="2" t="n">
-        <v>81</v>
-      </c>
-      <c r="X208" s="2" t="n">
-        <v>17.24</v>
-      </c>
-    </row>
-    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C209" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="D209" s="2"/>
-      <c r="E209" s="2"/>
-      <c r="F209" s="2"/>
-      <c r="G209" s="2"/>
-      <c r="W209" s="2" t="n">
-        <v>82</v>
-      </c>
-      <c r="X209" s="2" t="n">
-        <v>17.46</v>
-      </c>
-    </row>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C210" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="D210" s="2"/>
-      <c r="E210" s="2"/>
-      <c r="F210" s="2"/>
-      <c r="G210" s="2"/>
-      <c r="W210" s="2" t="n">
-        <v>83</v>
-      </c>
-      <c r="X210" s="2" t="n">
-        <v>17.68</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C211" s="2" t="n">
-        <v>26</v>
+        <v>170</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="D211" s="2"/>
       <c r="E211" s="2"/>
       <c r="F211" s="2"/>
       <c r="G211" s="2"/>
+      <c r="J211" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K211" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="M211" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="W211" s="2" t="n">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="X211" s="2" t="n">
-        <v>17.9</v>
+        <v>16.58</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="2" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C212" s="2" t="n">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
       <c r="W212" s="2" t="n">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="X212" s="2" t="n">
-        <v>18.12</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="2" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="C213" s="2" t="n">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
       <c r="F213" s="2"/>
       <c r="G213" s="2"/>
       <c r="W213" s="2" t="n">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="X213" s="2" t="n">
-        <v>18.34</v>
+        <v>17.02</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="2" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="C214" s="2" t="n">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D214" s="2"/>
       <c r="E214" s="2"/>
       <c r="F214" s="2"/>
       <c r="G214" s="2"/>
       <c r="W214" s="2" t="n">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="X214" s="2" t="n">
-        <v>18.56</v>
+        <v>17.24</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="2" t="s">
-        <v>169</v>
+        <v>60</v>
       </c>
       <c r="C215" s="2" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
       <c r="F215" s="2"/>
       <c r="G215" s="2"/>
       <c r="W215" s="2" t="n">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="X215" s="2" t="n">
-        <v>18.78</v>
+        <v>17.46</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="2" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="C216" s="2" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
       <c r="F216" s="2"/>
       <c r="G216" s="2"/>
       <c r="W216" s="2" t="n">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="X216" s="2" t="n">
-        <v>19</v>
+        <v>17.68</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C217" s="2" t="n">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D217" s="2"/>
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
       <c r="G217" s="2"/>
       <c r="W217" s="2" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="X217" s="2" t="n">
-        <v>19.22</v>
+        <v>17.9</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="2" t="s">
-        <v>172</v>
+        <v>64</v>
       </c>
       <c r="C218" s="2" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
       <c r="G218" s="2"/>
       <c r="W218" s="2" t="n">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="X218" s="2" t="n">
-        <v>19.44</v>
+        <v>18.12</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="s">
-        <v>173</v>
+        <v>65</v>
       </c>
       <c r="C219" s="2" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
       <c r="F219" s="2"/>
       <c r="G219" s="2"/>
       <c r="W219" s="2" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="X219" s="2" t="n">
-        <v>19.66</v>
+        <v>18.34</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="2" t="s">
-        <v>174</v>
+        <v>38</v>
       </c>
       <c r="C220" s="2" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
       <c r="F220" s="2"/>
       <c r="G220" s="2"/>
       <c r="W220" s="2" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="X220" s="2" t="n">
-        <v>19.88</v>
+        <v>18.56</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C221" s="2" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
       <c r="F221" s="2"/>
       <c r="G221" s="2"/>
       <c r="W221" s="2" t="n">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="X221" s="2" t="n">
-        <v>20.1</v>
+        <v>18.78</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C222" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
       <c r="W222" s="2" t="n">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="X222" s="2" t="n">
-        <v>20.32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C223" s="2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
       <c r="G223" s="2"/>
       <c r="W223" s="2" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="X223" s="2" t="n">
-        <v>20.54</v>
+        <v>19.22</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C224" s="2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
       <c r="G224" s="2"/>
       <c r="W224" s="2" t="n">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="X224" s="2" t="n">
-        <v>20.76</v>
+        <v>19.44</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C225" s="2" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
       <c r="W225" s="2" t="n">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="X225" s="2" t="n">
-        <v>20.98</v>
+        <v>19.66</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C226" s="2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
       <c r="G226" s="2"/>
       <c r="W226" s="2" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="X226" s="2" t="n">
-        <v>21.2</v>
+        <v>19.88</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="s">
-        <v>181</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="C227" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D227" s="2"/>
+      <c r="E227" s="2"/>
+      <c r="F227" s="2"/>
+      <c r="G227" s="2"/>
       <c r="W227" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="X227" s="2" t="n">
+        <v>20.1</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C228" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D228" s="2"/>
+      <c r="E228" s="2"/>
+      <c r="F228" s="2"/>
+      <c r="G228" s="2"/>
+      <c r="W228" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="X228" s="2" t="n">
+        <v>20.32</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C229" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D229" s="2"/>
+      <c r="E229" s="2"/>
+      <c r="F229" s="2"/>
+      <c r="G229" s="2"/>
+      <c r="W229" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="X229" s="2" t="n">
+        <v>20.54</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C230" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D230" s="2"/>
+      <c r="E230" s="2"/>
+      <c r="F230" s="2"/>
+      <c r="G230" s="2"/>
+      <c r="W230" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="X230" s="2" t="n">
+        <v>20.76</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C231" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D231" s="2"/>
+      <c r="E231" s="2"/>
+      <c r="F231" s="2"/>
+      <c r="G231" s="2"/>
+      <c r="W231" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="X231" s="2" t="n">
+        <v>20.98</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C232" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D232" s="2"/>
+      <c r="E232" s="2"/>
+      <c r="F232" s="2"/>
+      <c r="G232" s="2"/>
+      <c r="W232" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="X232" s="2" t="n">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="W233" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="X227" s="2" t="n">
+      <c r="X233" s="2" t="n">
         <v>21.42</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W228" s="2" t="n">
-        <v>101</v>
-      </c>
-      <c r="X228" s="2" t="n">
-        <v>21.64</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W229" s="2" t="n">
-        <v>102</v>
-      </c>
-      <c r="X229" s="2" t="n">
-        <v>21.86</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W230" s="2" t="n">
-        <v>103</v>
-      </c>
-      <c r="X230" s="2" t="n">
-        <v>22.08</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W231" s="2" t="n">
-        <v>104</v>
-      </c>
-      <c r="X231" s="2" t="n">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W232" s="2" t="n">
-        <v>105</v>
-      </c>
-      <c r="X232" s="2" t="n">
-        <v>22.52</v>
-      </c>
-    </row>
-    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W233" s="2" t="n">
-        <v>106</v>
-      </c>
-      <c r="X233" s="2" t="n">
-        <v>22.74</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W234" s="2" t="n">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="X234" s="2" t="n">
-        <v>22.96</v>
+        <v>21.64</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W235" s="2" t="n">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="X235" s="2" t="n">
-        <v>23.18</v>
+        <v>21.86</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W236" s="2" t="n">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="X236" s="2" t="n">
-        <v>23.4</v>
+        <v>22.08</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W237" s="2" t="n">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="X237" s="2" t="n">
-        <v>23.62</v>
+        <v>22.3</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W238" s="2" t="n">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="X238" s="2" t="n">
-        <v>23.84</v>
+        <v>22.52</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W239" s="2" t="n">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="X239" s="2" t="n">
-        <v>24.06</v>
+        <v>22.74</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W240" s="2" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="X240" s="2" t="n">
-        <v>24.28</v>
+        <v>22.96</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W241" s="2" t="n">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="X241" s="2" t="n">
-        <v>24.5</v>
+        <v>23.18</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W242" s="2" t="n">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="X242" s="2" t="n">
-        <v>24.72</v>
+        <v>23.4</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W243" s="2" t="n">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="X243" s="2" t="n">
-        <v>24.94</v>
+        <v>23.62</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W244" s="2" t="n">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="X244" s="2" t="n">
-        <v>25.16</v>
+        <v>23.84</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W245" s="2" t="n">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="X245" s="2" t="n">
-        <v>25.38</v>
+        <v>24.06</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W246" s="2" t="n">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="X246" s="2" t="n">
-        <v>25.6</v>
+        <v>24.28</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W247" s="2" t="n">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="X247" s="2" t="n">
-        <v>25.82</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W248" s="2" t="n">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="X248" s="2" t="n">
-        <v>26.04</v>
+        <v>24.72</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W249" s="2" t="n">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="X249" s="2" t="n">
-        <v>26.26</v>
+        <v>24.94</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W250" s="2" t="n">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="X250" s="2" t="n">
-        <v>26.48</v>
+        <v>25.16</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W251" s="2" t="n">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="X251" s="2" t="n">
-        <v>26.7</v>
+        <v>25.38</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W252" s="2" t="n">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="X252" s="2" t="n">
-        <v>26.92</v>
+        <v>25.6</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W253" s="2" t="n">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="X253" s="2" t="n">
-        <v>27.14</v>
+        <v>25.82</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W254" s="2" t="n">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="X254" s="2" t="n">
-        <v>27.36</v>
+        <v>26.04</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W255" s="2" t="n">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="X255" s="2" t="n">
-        <v>27.58</v>
+        <v>26.26</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W256" s="2" t="n">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="X256" s="2" t="n">
-        <v>27.8</v>
+        <v>26.48</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W257" s="2" t="n">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="X257" s="2" t="n">
-        <v>28.02</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W258" s="2" t="n">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="X258" s="2" t="n">
-        <v>28.24</v>
+        <v>26.92</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W259" s="2" t="n">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="X259" s="2" t="n">
-        <v>28.46</v>
+        <v>27.14</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W260" s="2" t="n">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="X260" s="2" t="n">
-        <v>28.68</v>
+        <v>27.36</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W261" s="2" t="n">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="X261" s="2" t="n">
-        <v>28.9</v>
+        <v>27.58</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W262" s="2" t="n">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="X262" s="2" t="n">
-        <v>29.12</v>
+        <v>27.8</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W263" s="2" t="n">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="X263" s="2" t="n">
-        <v>29.34</v>
+        <v>28.02</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W264" s="2" t="n">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="X264" s="2" t="n">
-        <v>29.56</v>
+        <v>28.24</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W265" s="2" t="n">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="X265" s="2" t="n">
-        <v>29.78</v>
+        <v>28.46</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W266" s="2" t="n">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="X266" s="2" t="n">
-        <v>30</v>
+        <v>28.68</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W267" s="2" t="n">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="X267" s="2" t="n">
-        <v>30.22</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W268" s="2" t="n">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="X268" s="2" t="n">
-        <v>30.44</v>
+        <v>29.12</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W269" s="2" t="n">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="X269" s="2" t="n">
-        <v>30.66</v>
+        <v>29.34</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W270" s="2" t="n">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="X270" s="2" t="n">
-        <v>30.88</v>
+        <v>29.56</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W271" s="2" t="n">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="X271" s="2" t="n">
-        <v>31.1</v>
+        <v>29.78</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W272" s="2" t="n">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="X272" s="2" t="n">
-        <v>31.32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W273" s="2" t="n">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="X273" s="2" t="n">
-        <v>31.54</v>
+        <v>30.22</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W274" s="2" t="n">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="X274" s="2" t="n">
-        <v>31.76</v>
+        <v>30.44</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W275" s="2" t="n">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="X275" s="2" t="n">
-        <v>31.98</v>
+        <v>30.66</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W276" s="2" t="n">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="X276" s="2" t="n">
-        <v>32.2</v>
+        <v>30.88</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W277" s="2" t="n">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="X277" s="2" t="n">
-        <v>32.42</v>
+        <v>31.1</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W278" s="2" t="n">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="X278" s="2" t="n">
-        <v>32.64</v>
+        <v>31.32</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W279" s="2" t="n">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="X279" s="2" t="n">
-        <v>32.86</v>
+        <v>31.54</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W280" s="2" t="n">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="X280" s="2" t="n">
-        <v>33.08</v>
+        <v>31.76</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W281" s="2" t="n">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="X281" s="2" t="n">
-        <v>33.3</v>
+        <v>31.98</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W282" s="2" t="n">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="X282" s="2" t="n">
-        <v>33.52</v>
+        <v>32.2</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W283" s="2" t="n">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="X283" s="2" t="n">
-        <v>33.74</v>
+        <v>32.42</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W284" s="2" t="n">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="X284" s="2" t="n">
-        <v>33.96</v>
+        <v>32.64</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W285" s="2" t="n">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="X285" s="2" t="n">
-        <v>34.18</v>
+        <v>32.86</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W286" s="2" t="n">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="X286" s="2" t="n">
-        <v>34.4</v>
+        <v>33.08</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W287" s="2" t="n">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="X287" s="2" t="n">
-        <v>34.62</v>
+        <v>33.3</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W288" s="2" t="n">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="X288" s="2" t="n">
-        <v>34.84</v>
+        <v>33.52</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W289" s="2" t="n">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="X289" s="2" t="n">
-        <v>35.06</v>
+        <v>33.74</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W290" s="2" t="n">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="X290" s="2" t="n">
-        <v>35.28</v>
+        <v>33.96</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W291" s="2" t="n">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="X291" s="2" t="n">
-        <v>35.5</v>
+        <v>34.18</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W292" s="2" t="n">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="X292" s="2" t="n">
-        <v>35.72</v>
+        <v>34.4</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W293" s="2" t="n">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="X293" s="2" t="n">
-        <v>35.94</v>
+        <v>34.62</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W294" s="2" t="n">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="X294" s="2" t="n">
-        <v>36.16</v>
+        <v>34.84</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W295" s="2" t="n">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="X295" s="2" t="n">
-        <v>36.38</v>
+        <v>35.06</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W296" s="2" t="n">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="X296" s="2" t="n">
-        <v>36.6</v>
+        <v>35.28</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W297" s="2" t="n">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="X297" s="2" t="n">
-        <v>36.82</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W298" s="2" t="n">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="X298" s="2" t="n">
-        <v>37.04</v>
+        <v>35.72</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W299" s="2" t="n">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="X299" s="2" t="n">
-        <v>37.26</v>
+        <v>35.94</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W300" s="2" t="n">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="X300" s="2" t="n">
-        <v>37.48</v>
+        <v>36.16</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W301" s="2" t="n">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="X301" s="2" t="n">
-        <v>37.7</v>
+        <v>36.38</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W302" s="2" t="n">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="X302" s="2" t="n">
-        <v>37.92</v>
+        <v>36.6</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W303" s="2" t="n">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="X303" s="2" t="n">
-        <v>38.14</v>
+        <v>36.82</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W304" s="2" t="n">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="X304" s="2" t="n">
-        <v>38.36</v>
+        <v>37.04</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W305" s="2" t="n">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="X305" s="2" t="n">
-        <v>38.58</v>
+        <v>37.26</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W306" s="2" t="n">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="X306" s="2" t="n">
-        <v>38.8</v>
+        <v>37.48</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W307" s="2" t="n">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="X307" s="2" t="n">
-        <v>39.02</v>
+        <v>37.7</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W308" s="2" t="n">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="X308" s="2" t="n">
-        <v>39.24</v>
+        <v>37.92</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W309" s="2" t="n">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="X309" s="2" t="n">
-        <v>39.46</v>
+        <v>38.14</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W310" s="2" t="n">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="X310" s="2" t="n">
-        <v>39.68</v>
+        <v>38.36</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W311" s="2" t="n">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="X311" s="2" t="n">
-        <v>39.9</v>
+        <v>38.58</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W312" s="2" t="n">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="X312" s="2" t="n">
-        <v>40.12</v>
+        <v>38.8</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W313" s="2" t="n">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="X313" s="2" t="n">
-        <v>40.34</v>
+        <v>39.02</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W314" s="2" t="n">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="X314" s="2" t="n">
-        <v>40.56</v>
+        <v>39.24</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W315" s="2" t="n">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="X315" s="2" t="n">
-        <v>40.78</v>
+        <v>39.46</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W316" s="2" t="n">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="X316" s="2" t="n">
-        <v>41</v>
+        <v>39.68</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W317" s="2" t="n">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="X317" s="2" t="n">
-        <v>41.22</v>
+        <v>39.9</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W318" s="2" t="n">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="X318" s="2" t="n">
-        <v>41.44</v>
+        <v>40.12</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W319" s="2" t="n">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="X319" s="2" t="n">
-        <v>41.66</v>
+        <v>40.34</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W320" s="2" t="n">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="X320" s="2" t="n">
-        <v>41.88</v>
+        <v>40.56</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W321" s="2" t="n">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="X321" s="2" t="n">
-        <v>42.1</v>
+        <v>40.78</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W322" s="2" t="n">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="X322" s="2" t="n">
-        <v>42.32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W323" s="2" t="n">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="X323" s="2" t="n">
-        <v>42.54</v>
+        <v>41.22</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W324" s="2" t="n">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="X324" s="2" t="n">
-        <v>42.76</v>
+        <v>41.44</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W325" s="2" t="n">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="X325" s="2" t="n">
-        <v>42.98</v>
+        <v>41.66</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W326" s="2" t="n">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="X326" s="2" t="n">
-        <v>43.2</v>
+        <v>41.88</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W327" s="2" t="n">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="X327" s="2" t="n">
-        <v>43.42</v>
+        <v>42.1</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W328" s="2" t="n">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="X328" s="2" t="n">
-        <v>43.64</v>
+        <v>42.32</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W329" s="2" t="n">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="X329" s="2" t="n">
-        <v>43.86</v>
+        <v>42.54</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W330" s="2" t="n">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="X330" s="2" t="n">
-        <v>44.08</v>
+        <v>42.76</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W331" s="2" t="n">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="X331" s="2" t="n">
-        <v>44.3</v>
+        <v>42.98</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W332" s="2" t="n">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="X332" s="2" t="n">
-        <v>44.52</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W333" s="2" t="n">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="X333" s="2" t="n">
-        <v>44.74</v>
+        <v>43.42</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W334" s="2" t="n">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="X334" s="2" t="n">
-        <v>44.96</v>
+        <v>43.64</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W335" s="2" t="n">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="X335" s="2" t="n">
-        <v>45.18</v>
+        <v>43.86</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W336" s="2" t="n">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="X336" s="2" t="n">
-        <v>45.4</v>
+        <v>44.08</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W337" s="2" t="n">
+        <v>204</v>
+      </c>
+      <c r="X337" s="2" t="n">
+        <v>44.3</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W338" s="2" t="n">
+        <v>205</v>
+      </c>
+      <c r="X338" s="2" t="n">
+        <v>44.52</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W339" s="2" t="n">
+        <v>206</v>
+      </c>
+      <c r="X339" s="2" t="n">
+        <v>44.74</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W340" s="2" t="n">
+        <v>207</v>
+      </c>
+      <c r="X340" s="2" t="n">
+        <v>44.96</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W341" s="2" t="n">
+        <v>208</v>
+      </c>
+      <c r="X341" s="2" t="n">
+        <v>45.18</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W342" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="X342" s="2" t="n">
+        <v>45.4</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W343" s="2" t="n">
         <v>210</v>
       </c>
-      <c r="X337" s="2" t="n">
+      <c r="X343" s="2" t="n">
         <v>45.62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished 2000 building setup and state slot error fix
</commit_message>
<xml_diff>
--- a/Modding resources/economy spreadsheets/size_modifier.xlsx
+++ b/Modding resources/economy spreadsheets/size_modifier.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="189">
   <si>
     <t>Name</t>
   </si>
@@ -719,36 +719,36 @@
   <dimension ref="A1:X343"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B129" activeCellId="0" sqref="B129"/>
+      <selection pane="bottomLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.6604651162791"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2744186046512"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.26046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.62790697674419"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.38604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.75348837209302"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="4.67441860465116"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.16744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.4139534883721"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.153488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.47441860465116"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.5209302325581"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="4.06046511627907"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="1" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="11.8139534883721"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="1" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="15.3813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3849,14 +3849,24 @@
       <c r="A79" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B79" s="0"/>
-      <c r="C79" s="0"/>
-      <c r="D79" s="0"/>
-      <c r="E79" s="0"/>
+      <c r="B79" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="F79" s="0"/>
       <c r="G79" s="0"/>
       <c r="H79" s="0"/>
-      <c r="I79" s="0"/>
+      <c r="I79" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="J79" s="0"/>
       <c r="K79" s="0"/>
       <c r="L79" s="0"/>
@@ -3905,7 +3915,9 @@
       <c r="A81" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B81" s="0"/>
+      <c r="B81" s="0" t="s">
+        <v>61</v>
+      </c>
       <c r="C81" s="0"/>
       <c r="D81" s="0"/>
       <c r="E81" s="0"/>
@@ -6147,7 +6159,9 @@
       <c r="A142" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="B142" s="0"/>
+      <c r="B142" s="0" t="s">
+        <v>61</v>
+      </c>
       <c r="C142" s="0"/>
       <c r="D142" s="0"/>
       <c r="E142" s="0"/>
@@ -6201,7 +6215,9 @@
       <c r="A144" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B144" s="0"/>
+      <c r="B144" s="0" t="s">
+        <v>61</v>
+      </c>
       <c r="C144" s="0"/>
       <c r="D144" s="0"/>
       <c r="E144" s="0"/>

</xml_diff>